<commit_message>
eia & ferc data updates, sdge rates. rate wide to tall
</commit_message>
<xml_diff>
--- a/Fig3_RateLevels/Consolidated Rate Info.xlsx
+++ b/Fig3_RateLevels/Consolidated Rate Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rayan/Developer/CCAResearch/ConsolidatedPrimerData/CA_electricity_primer/Fig3_RateLevels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D88296-3A58-544C-A0B5-289CFF9B2191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0107B5F9-2147-8144-B6EC-01875464D63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14080" activeTab="3" xr2:uid="{7039D85A-8A19-0F42-A262-787F6C9D5D5B}"/>
+    <workbookView xWindow="10580" yWindow="500" windowWidth="15020" windowHeight="14080" activeTab="3" xr2:uid="{7039D85A-8A19-0F42-A262-787F6C9D5D5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiered" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="151">
   <si>
     <t>LSE</t>
   </si>
@@ -479,6 +479,30 @@
   </si>
   <si>
     <t>PG&amp;E-2024</t>
+  </si>
+  <si>
+    <t>SGD&amp;E</t>
+  </si>
+  <si>
+    <t>SGDE</t>
+  </si>
+  <si>
+    <t>https://apps.openei.org/USURDB/rate/view/62f5346c75747b72641eb477#4__Fixed_Charges</t>
+  </si>
+  <si>
+    <t>TOU-DR1</t>
+  </si>
+  <si>
+    <t>DR</t>
+  </si>
+  <si>
+    <t>EVTOU</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Added: CCA generation, IOU distribution &amp; transmission, baseline incentive, franchise fee surcharge</t>
   </si>
 </sst>
 </file>
@@ -684,7 +708,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -772,13 +796,16 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -788,7 +815,16 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="44">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -3826,9 +3862,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'New-Tiered'!$A$2:$A$8</c:f>
+              <c:f>'New-Tiered'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>PG&amp;E</c:v>
                 </c:pt>
@@ -3849,16 +3885,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>PG&amp;E-2024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SGD&amp;E</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'New-Tiered'!$D$2:$D$8</c:f>
+              <c:f>'New-Tiered'!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>11.2836</c:v>
                 </c:pt>
@@ -3879,6 +3918,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>11.7501</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3915,9 +3957,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'New-Tiered'!$A$2:$A$8</c:f>
+              <c:f>'New-Tiered'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>PG&amp;E</c:v>
                 </c:pt>
@@ -3938,16 +3980,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>PG&amp;E-2024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SGD&amp;E</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'New-Tiered'!$E$2:$E$8</c:f>
+              <c:f>'New-Tiered'!$E$2:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3967,6 +4012,9 @@
                   <c:v>0.92999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4004,9 +4052,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'New-Tiered'!$A$2:$A$8</c:f>
+              <c:f>'New-Tiered'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>PG&amp;E</c:v>
                 </c:pt>
@@ -4027,16 +4075,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>PG&amp;E-2024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SGD&amp;E</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'New-Tiered'!$F$2:$F$8</c:f>
+              <c:f>'New-Tiered'!$F$2:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4056,6 +4107,9 @@
                   <c:v>0.92999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4093,9 +4147,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'New-Tiered'!$A$2:$A$8</c:f>
+              <c:f>'New-Tiered'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>PG&amp;E</c:v>
                 </c:pt>
@@ -4116,16 +4170,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>PG&amp;E-2024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SGD&amp;E</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'New-Tiered'!$G$2:$G$8</c:f>
+              <c:f>'New-Tiered'!$G$2:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4145,6 +4202,9 @@
                   <c:v>0.92999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4549,9 +4609,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>TOU!$A$2:$A$8</c:f>
+              <c:f>TOU!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>PG&amp;E</c:v>
                 </c:pt>
@@ -4572,16 +4632,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>PG&amp;E-2024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SDG&amp;E</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TOU!$D$2:$D$8</c:f>
+              <c:f>TOU!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>11.2836</c:v>
                 </c:pt>
@@ -4602,6 +4665,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>11.7501</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4638,9 +4704,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>TOU!$A$2:$A$8</c:f>
+              <c:f>TOU!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>PG&amp;E</c:v>
                 </c:pt>
@@ -4661,16 +4727,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>PG&amp;E-2024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SDG&amp;E</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TOU!$E$2:$E$8</c:f>
+              <c:f>TOU!$E$2:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4690,6 +4759,9 @@
                   <c:v>0.92999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5094,9 +5166,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'TOU-EV'!$A$2:$A$8</c:f>
+              <c:f>'TOU-EV'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>PG&amp;E</c:v>
                 </c:pt>
@@ -5117,16 +5189,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>PG&amp;E-2024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SDG&amp;E</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'TOU-EV'!$D$2:$D$8</c:f>
+              <c:f>'TOU-EV'!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>11.2836</c:v>
                 </c:pt>
@@ -5147,6 +5222,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>11.7501</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5183,9 +5261,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'TOU-EV'!$A$2:$A$8</c:f>
+              <c:f>'TOU-EV'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>PG&amp;E</c:v>
                 </c:pt>
@@ -5206,16 +5284,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>PG&amp;E-2024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SDG&amp;E</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'TOU-EV'!$E$2:$E$8</c:f>
+              <c:f>'TOU-EV'!$E$2:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5235,6 +5316,9 @@
                   <c:v>12.81</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -9706,64 +9790,65 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{622F9925-59E7-EF40-84D1-6E3283BE399E}" name="Table1" displayName="Table1" ref="A1:M8" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41" dataCellStyle="Currency">
-  <autoFilter ref="A1:M8" xr:uid="{622F9925-59E7-EF40-84D1-6E3283BE399E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{622F9925-59E7-EF40-84D1-6E3283BE399E}" name="Table1" displayName="Table1" ref="A1:M9" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" dataCellStyle="Currency">
+  <autoFilter ref="A1:M9" xr:uid="{622F9925-59E7-EF40-84D1-6E3283BE399E}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{ED67349A-8A4C-9E48-BEB1-46D207315EC5}" name="LSE" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{C2534D26-0176-BE43-A36D-642666F84B78}" name="Type" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{4BE4FD15-782C-3641-8E24-6E7DFD8EB062}" name="Rate Name" dataDxfId="38"/>
-    <tableColumn id="13" xr3:uid="{C0F46CEF-DCD0-BB47-B139-0EB002DDCBAD}" name="Minimum Charges ($/month)" dataDxfId="37" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{D0874B39-AD75-C446-A45A-8905FEB0E25A}" name="Fixed Charges Tier 1 ($/month)" dataDxfId="36" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{213136F0-A2F1-7E4E-9CB7-161C428CF1A9}" name="Fixed Charges Tier 2 ($/month)" dataDxfId="35" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{D937BE4E-031E-0444-9DA2-373CF38F5F0E}" name="Fixed Charges Tier 3 ($/month)" dataDxfId="34" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{2EE0018D-C87A-9B4F-813E-399127C712B1}" name="Tier 1 Rate ($/kWh)" dataDxfId="33" dataCellStyle="Currency"/>
-    <tableColumn id="8" xr3:uid="{D4E08105-A1AD-0C40-BC58-A06518FC8B81}" name="Tier 2 Rate ($/kWh)" dataDxfId="32" dataCellStyle="Currency"/>
-    <tableColumn id="9" xr3:uid="{AD005999-CA06-D548-9A48-04EE9C0BBF9C}" name="Tier 3 Rate ($/kWh)" dataDxfId="31" dataCellStyle="Currency"/>
-    <tableColumn id="10" xr3:uid="{0D31915C-674D-E04E-9284-E7F994346F47}" name="Tier 1 Amount Limit (kWh)" dataDxfId="30" dataCellStyle="Comma"/>
-    <tableColumn id="11" xr3:uid="{04D2C5F7-0956-AB48-B8BB-82314456C7E8}" name="Tier 2 Amount Limit (kWh)" dataDxfId="29" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{AB506B18-90B5-5C48-941E-FF8BC978622E}" name="Note" dataDxfId="28" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{ED67349A-8A4C-9E48-BEB1-46D207315EC5}" name="LSE" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{C2534D26-0176-BE43-A36D-642666F84B78}" name="Type" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{4BE4FD15-782C-3641-8E24-6E7DFD8EB062}" name="Rate Name" dataDxfId="39"/>
+    <tableColumn id="13" xr3:uid="{C0F46CEF-DCD0-BB47-B139-0EB002DDCBAD}" name="Minimum Charges ($/month)" dataDxfId="38" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{D0874B39-AD75-C446-A45A-8905FEB0E25A}" name="Fixed Charges Tier 1 ($/month)" dataDxfId="37" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{213136F0-A2F1-7E4E-9CB7-161C428CF1A9}" name="Fixed Charges Tier 2 ($/month)" dataDxfId="36" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{D937BE4E-031E-0444-9DA2-373CF38F5F0E}" name="Fixed Charges Tier 3 ($/month)" dataDxfId="35" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{2EE0018D-C87A-9B4F-813E-399127C712B1}" name="Tier 1 Rate ($/kWh)" dataDxfId="34" dataCellStyle="Currency"/>
+    <tableColumn id="8" xr3:uid="{D4E08105-A1AD-0C40-BC58-A06518FC8B81}" name="Tier 2 Rate ($/kWh)" dataDxfId="33" dataCellStyle="Currency"/>
+    <tableColumn id="9" xr3:uid="{AD005999-CA06-D548-9A48-04EE9C0BBF9C}" name="Tier 3 Rate ($/kWh)" dataDxfId="32" dataCellStyle="Currency"/>
+    <tableColumn id="10" xr3:uid="{0D31915C-674D-E04E-9284-E7F994346F47}" name="Tier 1 Amount Limit (kWh)" dataDxfId="31" dataCellStyle="Comma"/>
+    <tableColumn id="11" xr3:uid="{04D2C5F7-0956-AB48-B8BB-82314456C7E8}" name="Tier 2 Amount Limit (kWh)" dataDxfId="30" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{AB506B18-90B5-5C48-941E-FF8BC978622E}" name="Note" dataDxfId="29" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{49FA67C6-51F8-F342-87F4-DD10F5ADCB6B}" name="Table2" displayName="Table2" ref="A1:L8" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A1:L8" xr:uid="{49FA67C6-51F8-F342-87F4-DD10F5ADCB6B}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{31510521-DE32-3B4D-B619-FF2ED05955EC}" name="LSE" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{03D9D98B-2872-7D48-90F5-28FF6854553C}" name="Type" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{B8D8586E-F3BB-9245-B95A-AC600548C8A2}" name="Rate Name" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{34D838A8-7EA8-DC43-9BE5-0177C2694E62}" name="Minimum Charges ($/month)" dataDxfId="22" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{03783912-A703-0348-BB6F-12145C905895}" name="Fixed Charge ($/month)" dataDxfId="21" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{C0DD89ED-48CF-834B-9BB5-6148F49FA863}" name="Low Peak" dataDxfId="20" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{646F9F98-8DDC-CD4E-8D6E-8FE5EFBC5216}" name="Mid Peak" dataDxfId="19" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{C37FFE21-3145-F84E-A1A8-394D11C5091F}" name="Peak" dataDxfId="18" dataCellStyle="Currency"/>
-    <tableColumn id="8" xr3:uid="{2E823791-CF3C-114E-B67D-80EEA08D47ED}" name="Low Peak Hours" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{0051F9D1-C23A-CD43-B61A-E0AAFA8AF1D6}" name="Mid Peak Hours" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{1718EDE8-4368-3548-B154-711EB8BAC6A7}" name="Peak Hours" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{F84DB3D6-90B8-EE42-8623-4037379BA7EE}" name="Baseline credit" dataDxfId="14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{49FA67C6-51F8-F342-87F4-DD10F5ADCB6B}" name="Table2" displayName="Table2" ref="A1:M9" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+  <autoFilter ref="A1:M9" xr:uid="{49FA67C6-51F8-F342-87F4-DD10F5ADCB6B}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{31510521-DE32-3B4D-B619-FF2ED05955EC}" name="LSE" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{03D9D98B-2872-7D48-90F5-28FF6854553C}" name="Type" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{B8D8586E-F3BB-9245-B95A-AC600548C8A2}" name="Rate Name" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{34D838A8-7EA8-DC43-9BE5-0177C2694E62}" name="Minimum Charges ($/month)" dataDxfId="23" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{03783912-A703-0348-BB6F-12145C905895}" name="Fixed Charge ($/month)" dataDxfId="22" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{C0DD89ED-48CF-834B-9BB5-6148F49FA863}" name="Low Peak" dataDxfId="21" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{646F9F98-8DDC-CD4E-8D6E-8FE5EFBC5216}" name="Mid Peak" dataDxfId="20" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{C37FFE21-3145-F84E-A1A8-394D11C5091F}" name="Peak" dataDxfId="19" dataCellStyle="Currency"/>
+    <tableColumn id="8" xr3:uid="{2E823791-CF3C-114E-B67D-80EEA08D47ED}" name="Low Peak Hours" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{0051F9D1-C23A-CD43-B61A-E0AAFA8AF1D6}" name="Mid Peak Hours" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{1718EDE8-4368-3548-B154-711EB8BAC6A7}" name="Peak Hours" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{F84DB3D6-90B8-EE42-8623-4037379BA7EE}" name="Baseline credit" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{C4C439B2-D20A-3942-8AA0-6DAD2A6DA638}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34FCF372-FEAA-1341-90F1-F54CFE2E2B0B}" name="Table3" displayName="Table3" ref="A1:L8" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L8" xr:uid="{34FCF372-FEAA-1341-90F1-F54CFE2E2B0B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34FCF372-FEAA-1341-90F1-F54CFE2E2B0B}" name="Table3" displayName="Table3" ref="A1:L9" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:L9" xr:uid="{34FCF372-FEAA-1341-90F1-F54CFE2E2B0B}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{9C1B714A-42F7-4E4D-B344-DD609BAEA355}" name="LSE" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{87DF0F2F-BDDC-7744-A5E7-23288E96BE2C}" name="Type" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{45E06AEF-FA1B-7043-BAE4-198D776E8861}" name="Rate Name" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{9AA32FAE-99C6-1D48-A547-084E37A57CDE}" name="Minimum Charge ($/month)" dataDxfId="8" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{91B0AC90-0EFF-B64A-A54A-184A83940984}" name="Fixed Charge ($/month)" dataDxfId="7" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{EF365C78-8E71-9F40-84A4-CE7C7943AAD5}" name="Low Peak" dataDxfId="6" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{6D4DC051-49EF-C149-9123-CB9F09236D8E}" name="Mid Peak" dataDxfId="5" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{05BBCACD-4DCF-7145-BFCB-A60C180C4477}" name="Peak" dataDxfId="4" dataCellStyle="Currency"/>
-    <tableColumn id="8" xr3:uid="{290FFF60-FAD3-BD42-AB66-44CBDF1BE422}" name="Low Peak Hours" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{7E8D7913-3D63-3A4B-B286-885D9A8F5C29}" name="Mid Peak Hours" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{54084C43-EF71-5D4C-AE4F-F92FA99D885F}" name="Peak Hours" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{7E485E16-F5F8-B742-BFDE-0DE08B5A22F3}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9C1B714A-42F7-4E4D-B344-DD609BAEA355}" name="LSE" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{87DF0F2F-BDDC-7744-A5E7-23288E96BE2C}" name="Type" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{45E06AEF-FA1B-7043-BAE4-198D776E8861}" name="Rate Name" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{9AA32FAE-99C6-1D48-A547-084E37A57CDE}" name="Minimum Charge ($/month)" dataDxfId="9" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{91B0AC90-0EFF-B64A-A54A-184A83940984}" name="Fixed Charge ($/month)" dataDxfId="8" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{EF365C78-8E71-9F40-84A4-CE7C7943AAD5}" name="Low Peak" dataDxfId="7" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{6D4DC051-49EF-C149-9123-CB9F09236D8E}" name="Mid Peak" dataDxfId="6" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{05BBCACD-4DCF-7145-BFCB-A60C180C4477}" name="Peak" dataDxfId="5" dataCellStyle="Currency"/>
+    <tableColumn id="8" xr3:uid="{290FFF60-FAD3-BD42-AB66-44CBDF1BE422}" name="Low Peak Hours" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{7E8D7913-3D63-3A4B-B286-885D9A8F5C29}" name="Mid Peak Hours" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{54084C43-EF71-5D4C-AE4F-F92FA99D885F}" name="Peak Hours" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{7E485E16-F5F8-B742-BFDE-0DE08B5A22F3}" name="Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10865,10 +10950,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99CACCF-8A90-B745-8CE0-1BF96EFFA42E}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView zoomScale="113" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11197,40 +11282,76 @@
       </c>
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
-      <c r="M8" s="37">
+      <c r="M8" s="36">
         <v>45352</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" t="s">
-        <v>77</v>
-      </c>
+    <row r="9" spans="1:13" ht="17">
+      <c r="A9" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="18">
+        <f>0.35*30</f>
+        <v>10.5</v>
+      </c>
+      <c r="E9" s="18">
+        <v>0</v>
+      </c>
+      <c r="F9" s="18">
+        <v>0</v>
+      </c>
+      <c r="G9" s="18">
+        <v>0</v>
+      </c>
+      <c r="H9" s="18">
+        <v>0.45245000000000002</v>
+      </c>
+      <c r="I9" s="18">
+        <v>0.56969000000000003</v>
+      </c>
+      <c r="J9" s="18">
+        <v>0.56969000000000003</v>
+      </c>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="18"/>
     </row>
     <row r="11" spans="1:13">
+      <c r="A11" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="B12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="B13" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="B14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="B15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="B16" t="s">
         <v>117</v>
       </c>
     </row>
@@ -11245,18 +11366,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68462AF4-BB93-C948-8E27-561D7A5B2471}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="12" width="12.83203125" customWidth="1"/>
+    <col min="1" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="12" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="61" customHeight="1">
+    <row r="1" spans="1:13" ht="61" customHeight="1">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -11293,8 +11416,11 @@
       <c r="L1" s="25" t="s">
         <v>94</v>
       </c>
+      <c r="M1" s="38" t="s">
+        <v>149</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="20" customHeight="1">
+    <row r="2" spans="1:13" ht="20" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>39</v>
       </c>
@@ -11332,8 +11458,9 @@
       <c r="L2" s="12">
         <v>-8.3210000000000006E-2</v>
       </c>
+      <c r="M2" s="37"/>
     </row>
-    <row r="3" spans="1:12" ht="20" customHeight="1">
+    <row r="3" spans="1:13" ht="20" customHeight="1">
       <c r="A3" s="12" t="s">
         <v>36</v>
       </c>
@@ -11375,8 +11502,9 @@
       <c r="L3" s="26">
         <v>-9.3909999999999993E-2</v>
       </c>
+      <c r="M3" s="37"/>
     </row>
-    <row r="4" spans="1:12" ht="20" customHeight="1">
+    <row r="4" spans="1:13" ht="20" customHeight="1">
       <c r="A4" s="12" t="s">
         <v>20</v>
       </c>
@@ -11411,8 +11539,9 @@
         <v>103</v>
       </c>
       <c r="L4" s="12"/>
+      <c r="M4" s="37"/>
     </row>
-    <row r="5" spans="1:12" ht="20" customHeight="1">
+    <row r="5" spans="1:13" ht="20" customHeight="1">
       <c r="A5" s="12" t="s">
         <v>18</v>
       </c>
@@ -11447,8 +11576,9 @@
         <v>108</v>
       </c>
       <c r="L5" s="12"/>
+      <c r="M5" s="37"/>
     </row>
-    <row r="6" spans="1:12" ht="20" customHeight="1">
+    <row r="6" spans="1:13" ht="20" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>74</v>
       </c>
@@ -11467,15 +11597,15 @@
         <v>0</v>
       </c>
       <c r="F6" s="18">
-        <f>0.144+0.05254+0.00059+0.00069+0.02554+0.00135+0.00346+0.00254+0.12646-0.00071+0.0053+0.0003+0.00289+0.06047</f>
-        <v>0.42542000000000008</v>
+        <f>0.144+0.05254+0.00059+0.00069+0.02554+0.00135+0.00346+0.00254+0.12646-0.00071+0.0053+0.0003+0.00289+0.06047+0.00111</f>
+        <v>0.42653000000000008</v>
       </c>
       <c r="G6" s="18" t="s">
         <v>64</v>
       </c>
       <c r="H6" s="18">
-        <f>0.195+0.05254+0.00059+0.00069+0.02554+0.00135+0.00346+0.00254+0.14646-0.00071+0.0053+0.0003+0.00289+0.06047</f>
-        <v>0.49642000000000014</v>
+        <f>0.195+0.05254+0.00059+0.00069+0.02554+0.00135+0.00346+0.00254+0.14646-0.00071+0.0053+0.0003+0.00289+0.06047+0.00111</f>
+        <v>0.49753000000000014</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -11483,8 +11613,11 @@
       <c r="L6" s="12">
         <v>-8.3210000000000006E-2</v>
       </c>
+      <c r="M6" s="37" t="s">
+        <v>150</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" ht="20" customHeight="1">
+    <row r="7" spans="1:13" ht="20" customHeight="1">
       <c r="A7" s="12" t="s">
         <v>75</v>
       </c>
@@ -11526,41 +11659,75 @@
       <c r="L7" s="26">
         <v>-9.3909999999999993E-2</v>
       </c>
+      <c r="M7" s="37"/>
     </row>
-    <row r="8" spans="1:12" ht="17">
-      <c r="A8" s="35" t="s">
+    <row r="8" spans="1:13" ht="17">
+      <c r="A8" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="12" t="s">
         <v>121</v>
       </c>
       <c r="D8" s="18">
         <f>0.39167*30</f>
         <v>11.7501</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="35">
         <v>0</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="35">
         <v>0.53605000000000003</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8" s="35">
         <v>0.61948999999999999</v>
       </c>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35">
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12">
         <v>-0.10607</v>
       </c>
+      <c r="M8" s="37"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="9" spans="1:13" ht="17">
+      <c r="A9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="18">
+        <f>0.38*30</f>
+        <v>11.4</v>
+      </c>
+      <c r="E9" s="35">
+        <v>0</v>
+      </c>
+      <c r="F9" s="35">
+        <v>0.35515000000000002</v>
+      </c>
+      <c r="G9" s="35">
+        <v>0.51978999999999997</v>
+      </c>
+      <c r="H9" s="35">
+        <v>0.83325000000000005</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="37"/>
+    </row>
+    <row r="10" spans="1:13">
       <c r="F10" s="30"/>
     </row>
   </sheetData>
@@ -11573,10 +11740,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B05EA0-08D1-1640-B22C-5644B087CE35}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11797,13 +11964,16 @@
         <v>0</v>
       </c>
       <c r="F6" s="18">
-        <v>0.128</v>
+        <f>0.128+0.02597+0.05254 +0.00059+0.00069+0.02554+0.00135 +0.0003+0.0053+0.00346+0.00254 -0.00071+0.00289+0.00111</f>
+        <v>0.24956999999999999</v>
       </c>
       <c r="G6" s="18">
-        <v>0.16700000000000001</v>
+        <f>0.167+0.18684+0.05254 +0.00059+0.00069+0.02554+0.00135 +0.0003+0.0053+0.00346+0.00254 -0.00071+0.00289+0.00111</f>
+        <v>0.44944000000000017</v>
       </c>
       <c r="H6" s="18">
-        <v>0.21</v>
+        <f>0.21+0.25262+0.05254 +0.00059+0.00069+0.02554+0.00135 +0.0003+0.0053+0.00346+0.00254 -0.00071+0.00289+0.00111</f>
+        <v>0.55821999999999994</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>85</v>
@@ -11858,35 +12028,66 @@
       <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:12" ht="17">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="12" t="s">
         <v>120</v>
       </c>
       <c r="D8" s="18">
         <f>0.39167*30</f>
         <v>11.7501</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="35">
         <v>0</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="35">
         <v>0.34577999999999998</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="35">
         <v>0.54779</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8" s="35">
         <v>0.65827999999999998</v>
       </c>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+    </row>
+    <row r="9" spans="1:12" ht="17">
+      <c r="A9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" s="18">
+        <f>0.38 *30</f>
+        <v>11.4</v>
+      </c>
+      <c r="E9" s="35">
+        <v>0</v>
+      </c>
+      <c r="F9" s="35">
+        <v>0.2848</v>
+      </c>
+      <c r="G9" s="35">
+        <v>0.49726999999999999</v>
+      </c>
+      <c r="H9" s="35">
+        <v>0.83226999999999995</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11914,10 +12115,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5AEDE0-E5EA-EC47-AA3E-9D4F2CB3BBF1}">
-  <dimension ref="A2:E7"/>
+  <dimension ref="A2:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11983,6 +12184,14 @@
       </c>
       <c r="B7" s="6" t="s">
         <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added FF to tiered rates, created res rate time series, consolidated JRC data
</commit_message>
<xml_diff>
--- a/Fig3_RateLevels/Consolidated Rate Info.xlsx
+++ b/Fig3_RateLevels/Consolidated Rate Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rayan/Developer/CCAResearch/ConsolidatedPrimerData/CA_electricity_primer/Fig3_RateLevels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0107B5F9-2147-8144-B6EC-01875464D63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0833F2ED-06B9-FD40-8062-7DCF36C63C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10580" yWindow="500" windowWidth="15020" windowHeight="14080" activeTab="3" xr2:uid="{7039D85A-8A19-0F42-A262-787F6C9D5D5B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{7039D85A-8A19-0F42-A262-787F6C9D5D5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiered" sheetId="1" r:id="rId1"/>
@@ -424,12 +424,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>I have taken the CPA generation rate, added the SCE D delivery rate, subtracted the SCE D WTC component, and added the SCE CCA-CRS WTC, FRC, and PCIA components</t>
-  </si>
-  <si>
-    <t>I have taken the MCE generation rate, added the PG&amp;E E-1 delivery rate and incentive adjustment components except for WFC, PCIA, ECRA, and CTC, from the E1 sheet. I have added WFC, PCIA, ECRA, and CTC from the CCA-CRS.</t>
-  </si>
-  <si>
     <t>https://www.pge.com/tariffs/assets/pdf/adviceletter/ELEC_6946-E.pdf</t>
   </si>
   <si>
@@ -503,6 +497,12 @@
   </si>
   <si>
     <t>Added: CCA generation, IOU distribution &amp; transmission, baseline incentive, franchise fee surcharge</t>
+  </si>
+  <si>
+    <t>I have taken the CPA generation rate, added the SCE D delivery rate, subtracted the SCE D WTC component, and added the SCE CCA-CRS WTC, FRC, and PCIA and FF components</t>
+  </si>
+  <si>
+    <t>I have taken the MCE generation rate, added the PG&amp;E E-1 delivery rate and incentive adjustment components except for WFC, PCIA, ECRA, and CTC, from the E1 sheet. I have added WFC, PCIA, ECRA, and CTC from the CCA-CRS.I have added the FF from the E-FFS,</t>
   </si>
 </sst>
 </file>
@@ -708,7 +708,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -802,10 +802,7 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -816,15 +813,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="44">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -970,6 +958,15 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -9827,28 +9824,28 @@
     <tableColumn id="9" xr3:uid="{0051F9D1-C23A-CD43-B61A-E0AAFA8AF1D6}" name="Mid Peak Hours" dataDxfId="17"/>
     <tableColumn id="10" xr3:uid="{1718EDE8-4368-3548-B154-711EB8BAC6A7}" name="Peak Hours" dataDxfId="16"/>
     <tableColumn id="11" xr3:uid="{F84DB3D6-90B8-EE42-8623-4037379BA7EE}" name="Baseline credit" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{C4C439B2-D20A-3942-8AA0-6DAD2A6DA638}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{C4C439B2-D20A-3942-8AA0-6DAD2A6DA638}" name="Column1" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34FCF372-FEAA-1341-90F1-F54CFE2E2B0B}" name="Table3" displayName="Table3" ref="A1:L9" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34FCF372-FEAA-1341-90F1-F54CFE2E2B0B}" name="Table3" displayName="Table3" ref="A1:L9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:L9" xr:uid="{34FCF372-FEAA-1341-90F1-F54CFE2E2B0B}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{9C1B714A-42F7-4E4D-B344-DD609BAEA355}" name="LSE" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{87DF0F2F-BDDC-7744-A5E7-23288E96BE2C}" name="Type" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{45E06AEF-FA1B-7043-BAE4-198D776E8861}" name="Rate Name" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{9AA32FAE-99C6-1D48-A547-084E37A57CDE}" name="Minimum Charge ($/month)" dataDxfId="9" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{91B0AC90-0EFF-B64A-A54A-184A83940984}" name="Fixed Charge ($/month)" dataDxfId="8" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{EF365C78-8E71-9F40-84A4-CE7C7943AAD5}" name="Low Peak" dataDxfId="7" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{6D4DC051-49EF-C149-9123-CB9F09236D8E}" name="Mid Peak" dataDxfId="6" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{05BBCACD-4DCF-7145-BFCB-A60C180C4477}" name="Peak" dataDxfId="5" dataCellStyle="Currency"/>
-    <tableColumn id="8" xr3:uid="{290FFF60-FAD3-BD42-AB66-44CBDF1BE422}" name="Low Peak Hours" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{7E8D7913-3D63-3A4B-B286-885D9A8F5C29}" name="Mid Peak Hours" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{54084C43-EF71-5D4C-AE4F-F92FA99D885F}" name="Peak Hours" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{7E485E16-F5F8-B742-BFDE-0DE08B5A22F3}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{9C1B714A-42F7-4E4D-B344-DD609BAEA355}" name="LSE" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{87DF0F2F-BDDC-7744-A5E7-23288E96BE2C}" name="Type" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{45E06AEF-FA1B-7043-BAE4-198D776E8861}" name="Rate Name" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{9AA32FAE-99C6-1D48-A547-084E37A57CDE}" name="Minimum Charge ($/month)" dataDxfId="8" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{91B0AC90-0EFF-B64A-A54A-184A83940984}" name="Fixed Charge ($/month)" dataDxfId="7" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{EF365C78-8E71-9F40-84A4-CE7C7943AAD5}" name="Low Peak" dataDxfId="6" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{6D4DC051-49EF-C149-9123-CB9F09236D8E}" name="Mid Peak" dataDxfId="5" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{05BBCACD-4DCF-7145-BFCB-A60C180C4477}" name="Peak" dataDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="8" xr3:uid="{290FFF60-FAD3-BD42-AB66-44CBDF1BE422}" name="Low Peak Hours" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{7E8D7913-3D63-3A4B-B286-885D9A8F5C29}" name="Mid Peak Hours" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{54084C43-EF71-5D4C-AE4F-F92FA99D885F}" name="Peak Hours" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{7E485E16-F5F8-B742-BFDE-0DE08B5A22F3}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10953,12 +10950,13 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="12" width="12.83203125" customWidth="1"/>
+    <col min="13" max="13" width="42.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="91" customHeight="1">
@@ -10972,25 +10970,25 @@
         <v>47</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E1" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="I1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>136</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>138</v>
       </c>
       <c r="K1" s="17" t="s">
         <v>78</v>
@@ -11187,21 +11185,21 @@
         <v>0</v>
       </c>
       <c r="H6" s="18">
-        <f>0.149-0.03584+0.12203+0.05254+0.00059+0.00069+0.02554+0.00135+0.00346+0.00254+0.00798-0.00798-0.00071+0.0053+0.0003+0.00289</f>
-        <v>0.32968000000000014</v>
+        <f>0.149-0.03584+0.12203+0.05254+0.00059+0.00069+0.02554+0.00135+0.00346+0.00254+0.00798-0.00798-0.00071+0.0053+0.0003+0.00289+0.00111</f>
+        <v>0.33079000000000014</v>
       </c>
       <c r="I6" s="18">
-        <f>0.149+0.04882+0.12203+0.05254+0.00059+0.00069+0.02554+0.00135+0.00346+0.00254+0.00798-0.00798-0.00071+0.0053+0.0003+0.00289</f>
-        <v>0.4143400000000001</v>
+        <f>0.149+0.04882+0.12203+0.05254+0.00059+0.00069+0.02554+0.00135+0.00346+0.00254+0.00798-0.00798-0.00071+0.0053+0.0003+0.00289+0.00111</f>
+        <v>0.4154500000000001</v>
       </c>
       <c r="J6" s="18">
         <f>Table1[[#This Row],[Tier 2 Rate ($/kWh)]]</f>
-        <v>0.4143400000000001</v>
+        <v>0.4154500000000001</v>
       </c>
       <c r="K6" s="20"/>
       <c r="L6" s="20"/>
       <c r="M6" s="18" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="20" customHeight="1">
@@ -11245,12 +11243,12 @@
       <c r="K7" s="20"/>
       <c r="L7" s="20"/>
       <c r="M7" s="18" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="17">
       <c r="A8" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>37</v>
@@ -11288,13 +11286,13 @@
     </row>
     <row r="9" spans="1:13" ht="17">
       <c r="A9" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D9" s="18">
         <f>0.35*30</f>
@@ -11368,8 +11366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68462AF4-BB93-C948-8E27-561D7A5B2471}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11390,19 +11388,19 @@
         <v>47</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F1" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>141</v>
       </c>
       <c r="I1" s="24" t="s">
         <v>80</v>
@@ -11416,8 +11414,8 @@
       <c r="L1" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="38" t="s">
-        <v>149</v>
+      <c r="M1" s="37" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="20" customHeight="1">
@@ -11458,7 +11456,7 @@
       <c r="L2" s="12">
         <v>-8.3210000000000006E-2</v>
       </c>
-      <c r="M2" s="37"/>
+      <c r="M2" s="12"/>
     </row>
     <row r="3" spans="1:13" ht="20" customHeight="1">
       <c r="A3" s="12" t="s">
@@ -11502,7 +11500,7 @@
       <c r="L3" s="26">
         <v>-9.3909999999999993E-2</v>
       </c>
-      <c r="M3" s="37"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:13" ht="20" customHeight="1">
       <c r="A4" s="12" t="s">
@@ -11539,7 +11537,7 @@
         <v>103</v>
       </c>
       <c r="L4" s="12"/>
-      <c r="M4" s="37"/>
+      <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:13" ht="20" customHeight="1">
       <c r="A5" s="12" t="s">
@@ -11576,7 +11574,7 @@
         <v>108</v>
       </c>
       <c r="L5" s="12"/>
-      <c r="M5" s="37"/>
+      <c r="M5" s="12"/>
     </row>
     <row r="6" spans="1:13" ht="20" customHeight="1">
       <c r="A6" s="12" t="s">
@@ -11613,8 +11611,8 @@
       <c r="L6" s="12">
         <v>-8.3210000000000006E-2</v>
       </c>
-      <c r="M6" s="37" t="s">
-        <v>150</v>
+      <c r="M6" s="12" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="20" customHeight="1">
@@ -11659,11 +11657,11 @@
       <c r="L7" s="26">
         <v>-9.3909999999999993E-2</v>
       </c>
-      <c r="M7" s="37"/>
+      <c r="M7" s="12"/>
     </row>
     <row r="8" spans="1:13" ht="17">
       <c r="A8" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>37</v>
@@ -11693,7 +11691,7 @@
       <c r="L8" s="12">
         <v>-0.10607</v>
       </c>
-      <c r="M8" s="37"/>
+      <c r="M8" s="12"/>
     </row>
     <row r="9" spans="1:13" ht="17">
       <c r="A9" s="12" t="s">
@@ -11703,7 +11701,7 @@
         <v>37</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D9" s="18">
         <f>0.38*30</f>
@@ -11725,7 +11723,7 @@
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
-      <c r="M9" s="37"/>
+      <c r="M9" s="12"/>
     </row>
     <row r="10" spans="1:13">
       <c r="F10" s="30"/>
@@ -11742,8 +11740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B05EA0-08D1-1640-B22C-5644B087CE35}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11762,19 +11760,19 @@
         <v>47</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F1" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>139</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>141</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>80</v>
@@ -11865,7 +11863,7 @@
         <v>97</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="20" customHeight="1">
@@ -12029,7 +12027,7 @@
     </row>
     <row r="8" spans="1:12" ht="17">
       <c r="A8" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>37</v>
@@ -12066,7 +12064,7 @@
         <v>37</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D9" s="18">
         <f>0.38 *30</f>
@@ -12131,10 +12129,10 @@
         <v>87</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12167,7 +12165,7 @@
         <v>104</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -12188,10 +12186,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>